<commit_message>
Refactorisation complète du code... Début mise en place remplissage PDF
</commit_message>
<xml_diff>
--- a/donnees/listesAdherents/2025.xlsx
+++ b/donnees/listesAdherents/2025.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -78,11 +80,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -449,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,213 +460,196 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="16" customWidth="1" min="1" max="1"/>
-    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="5" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="8" customWidth="1" min="8" max="8"/>
-    <col width="25" customWidth="1" min="9" max="9"/>
-    <col width="10" customWidth="1" min="10" max="10"/>
-    <col width="25" customWidth="1" min="11" max="11"/>
-    <col width="15" customWidth="1" min="12" max="12"/>
+    <col width="5" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="8" customWidth="1" min="12" max="12"/>
     <col width="8" customWidth="1" min="13" max="13"/>
     <col width="8" customWidth="1" min="14" max="14"/>
     <col width="8" customWidth="1" min="15" max="15"/>
     <col width="8" customWidth="1" min="16" max="16"/>
-    <col width="8" customWidth="1" min="17" max="17"/>
-    <col width="15" customWidth="1" min="18" max="18"/>
-    <col width="10" customWidth="1" min="19" max="19"/>
-    <col width="20" customWidth="1" min="20" max="20"/>
+    <col width="15" customWidth="1" min="17" max="17"/>
+    <col width="10" customWidth="1" min="18" max="18"/>
+    <col width="20" customWidth="1" min="19" max="19"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Enregistrement</t>
+          <t>Adresse mail</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Adresse mail</t>
+          <t>Nom</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Nom</t>
+          <t>Prenom</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Prenom</t>
+          <t>IDs reçus</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>IDs reçus</t>
+          <t>Statut</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Statut</t>
+          <t>Date dernière adhésion</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Date dernière adhésion</t>
+          <t>Envoi mails</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Envoi mails</t>
+          <t>Adresse</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Adresse</t>
+          <t>Code postal</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Code postal</t>
+          <t>Ville</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Ville</t>
+          <t>Téléphone</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Téléphone</t>
+          <t>Montant adhésion payé année n-1</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Montant adhésion payé année n-1</t>
+          <t>Montant adhésion année n</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Montant adhésion année n</t>
+          <t>Montant adhésion année n+1</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Montant adhésion année n+1</t>
+          <t>Montant dons année n</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Montant dons année n</t>
+          <t>Total année n</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Total année n</t>
+          <t>Dernier paiement</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Dernier paiement</t>
+          <t>Dern. moy. paiement</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Dern. moy. paiement</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Remarques</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>04/08/2024</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>0ddd9@test.fr</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Lesage</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Henri</t>
         </is>
       </c>
-      <c r="E2" s="2" t="n"/>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr"/>
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>RA</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>2024</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>Oui</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="G2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3" t="inlineStr">
         <is>
           <t>9 allée des lagomorphes</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="I2" s="3" t="inlineStr">
         <is>
           <t>38600</t>
         </is>
       </c>
-      <c r="K2" s="2" t="inlineStr">
+      <c r="J2" s="3" t="inlineStr">
         <is>
           <t>Fontaine</t>
         </is>
       </c>
-      <c r="L2" s="2" t="n"/>
-      <c r="M2" s="2" t="n">
+      <c r="K2" s="3" t="inlineStr"/>
+      <c r="L2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="N2" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="O2" s="2" t="n">
+      <c r="M2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="P2" s="2" t="n">
+      <c r="N2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="R2" s="2" t="inlineStr">
+      <c r="O2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3" t="inlineStr">
         <is>
           <t>01/05/2025</t>
         </is>
       </c>
-      <c r="S2" s="2" t="inlineStr">
+      <c r="R2" s="3" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="T2" s="2" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="S2" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>